<commit_message>
Update column titles of data to make consistent.
</commit_message>
<xml_diff>
--- a/hospitalized_covid/Israeli_data_August_15_2021 original.xlsx
+++ b/hospitalized_covid/Israeli_data_August_15_2021 original.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsmorris/Box/A_Penn/Coronavirus/website/vaccineas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/lawrennd/datasets_mirror/hospitalized_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB163127-894A-7541-AEED-DD4B23CF824C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B9710-7BE6-F444-8F79-5C49664772ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-72360" yWindow="8960" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="4160" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="חולים פעילים - גיל והתחסנות..." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>קבוצת גיל</t>
   </si>
@@ -97,24 +108,15 @@
     <t>Active patients -- age and immunization</t>
   </si>
   <si>
-    <t>not vax</t>
-  </si>
-  <si>
     <t>vax</t>
   </si>
   <si>
     <t>partial vax</t>
   </si>
   <si>
-    <t>not vax per 100k</t>
-  </si>
-  <si>
     <t>vax per 100k</t>
   </si>
   <si>
-    <t>partial vax 100k</t>
-  </si>
-  <si>
     <t>severe unvax</t>
   </si>
   <si>
@@ -127,13 +129,19 @@
     <t>severe unvax per 100k</t>
   </si>
   <si>
-    <t>severe vax 100k</t>
-  </si>
-  <si>
-    <t>severe parital vax per 1`00k</t>
-  </si>
-  <si>
-    <t>risk severe 20-29</t>
+    <t>partial vax per 100k</t>
+  </si>
+  <si>
+    <t>severe parital vax per 100k</t>
+  </si>
+  <si>
+    <t>unvax per 100k</t>
+  </si>
+  <si>
+    <t>unvax</t>
+  </si>
+  <si>
+    <t>severe vax per 100k</t>
   </si>
 </sst>
 </file>
@@ -141,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -176,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -517,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,19 +539,19 @@
     <col min="7" max="7" width="15.5" style="3" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" customWidth="1"/>
     <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="12" width="20.83203125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="23.5" style="4" customWidth="1"/>
-    <col min="14" max="14" width="26.5" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="20.83203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="23.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="26.5" style="4" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -577,58 +585,55 @@
       <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="M2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -663,17 +668,13 @@
         <v>0.3</v>
       </c>
       <c r="L4" s="4">
-        <f>K4/K7</f>
-        <v>4.8387096774193547E-2</v>
+        <v>0</v>
       </c>
       <c r="M4" s="4">
         <v>0</v>
       </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -708,17 +709,13 @@
         <v>1.6</v>
       </c>
       <c r="L5" s="4">
-        <f>K5/K7</f>
-        <v>0.25806451612903225</v>
+        <v>0</v>
       </c>
       <c r="M5" s="4">
         <v>0</v>
       </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -753,17 +750,13 @@
         <v>1.5</v>
       </c>
       <c r="L6" s="4">
-        <f>K6/K7</f>
-        <v>0.24193548387096772</v>
+        <v>0</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
       </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -798,16 +791,13 @@
         <v>6.2</v>
       </c>
       <c r="L7" s="4">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="M7" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -842,17 +832,13 @@
         <v>16.5</v>
       </c>
       <c r="L8" s="4">
-        <f>K8/K7</f>
-        <v>2.661290322580645</v>
+        <v>1</v>
       </c>
       <c r="M8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" s="4">
         <v>3.8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -887,17 +873,13 @@
         <v>40.200000000000003</v>
       </c>
       <c r="L9" s="4">
-        <f>K9/K7</f>
-        <v>6.4838709677419359</v>
+        <v>2.9</v>
       </c>
       <c r="M9" s="4">
-        <v>2.9</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -932,17 +914,13 @@
         <v>76.7</v>
       </c>
       <c r="L10" s="4">
-        <f>K10/K7</f>
-        <v>12.370967741935484</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="M10" s="4">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="N10" s="4">
         <v>28.1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -977,17 +955,13 @@
         <v>190.1</v>
       </c>
       <c r="L11" s="4">
-        <f>K11/K7</f>
-        <v>30.661290322580644</v>
+        <v>19.8</v>
       </c>
       <c r="M11" s="4">
-        <v>19.8</v>
-      </c>
-      <c r="N11" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1022,17 +996,13 @@
         <v>252.3</v>
       </c>
       <c r="L12" s="4">
-        <f>K12/K7</f>
-        <v>40.693548387096776</v>
+        <v>47.9</v>
       </c>
       <c r="M12" s="4">
-        <v>47.9</v>
-      </c>
-      <c r="N12" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1067,13 +1037,9 @@
         <v>510.9</v>
       </c>
       <c r="L13" s="4">
-        <f>K13/K7</f>
-        <v>82.403225806451601</v>
+        <v>38.6</v>
       </c>
       <c r="M13" s="4">
-        <v>38.6</v>
-      </c>
-      <c r="N13" s="4">
         <v>113.4</v>
       </c>
     </row>
@@ -1095,7 +1061,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="M4:N13 M1:N2 H1:J2 H4:J13 B4:G13 B2:G2 B1:G1 A2 A4:A13 K1:K2 K4:K13" numberStoredAsText="1"/>
+    <ignoredError sqref="L4:M13 L1:M2 H1:J2 H4:J13 B4:G13 B2:G2 B1:G1 A2 A4:A13 K1:K2 K4:K13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>